<commit_message>
Installers for both MATLAB App and Stand Alone with the documentation
</commit_message>
<xml_diff>
--- a/docs/_site/pages/tutorial/start_new_analysis/media/demo/excel_files/demo_analysis_results.xlsx
+++ b/docs/_site/pages/tutorial/start_new_analysis/media/demo/excel_files/demo_analysis_results.xlsx
@@ -17412,10 +17412,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="H2" s="0">
         <v>0.10000000000000001</v>
-      </c>
-      <c r="H2" s="0">
-        <v>0.0001</v>
       </c>
       <c r="I2" s="0">
         <v>0</v>
@@ -17427,7 +17427,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="0">
-        <v>1945372.1693544229</v>
+        <v>1879084.1695828021</v>
       </c>
       <c r="M2" s="0">
         <v>92.316930775646341</v>
@@ -17448,10 +17448,10 @@
         <v>1</v>
       </c>
       <c r="S2" s="0">
-        <v>0.98296636307425411</v>
+        <v>0.99469202965947223</v>
       </c>
       <c r="T2" s="0">
-        <v>281697.56203156873</v>
+        <v>316190.70182045136</v>
       </c>
       <c r="U2" s="0">
         <v>0</v>
@@ -18285,13 +18285,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>1.368566191124886e-14</v>
+        <v>3.8408873234104569e-14</v>
       </c>
       <c r="D2" s="0">
-        <v>17719.477896618617</v>
+        <v>17566.277658747586</v>
       </c>
       <c r="E2" s="0">
-        <v>1.368566191124886e-14</v>
+        <v>3.8408873234104569e-14</v>
       </c>
       <c r="F2" s="0"/>
     </row>
@@ -18303,13 +18303,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="0">
-        <v>4.8348543086757017e-14</v>
+        <v>1.3186848911070809e-13</v>
       </c>
       <c r="D3" s="0">
-        <v>17686.249374959985</v>
+        <v>17525.896620416133</v>
       </c>
       <c r="E3" s="0">
-        <v>4.8348543086757017e-14</v>
+        <v>1.3186848911070809e-13</v>
       </c>
       <c r="F3" s="0"/>
     </row>
@@ -18321,13 +18321,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>1.6752011387239575e-13</v>
+        <v>4.4421950115899592e-13</v>
       </c>
       <c r="D4" s="0">
-        <v>17653.020853301354</v>
+        <v>17485.515582084681</v>
       </c>
       <c r="E4" s="0">
-        <v>1.6752011387239575e-13</v>
+        <v>4.4421950115899592e-13</v>
       </c>
       <c r="F4" s="0"/>
     </row>
@@ -18339,13 +18339,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="0">
-        <v>5.6926765740946833e-13</v>
+        <v>1.4682544855635949e-12</v>
       </c>
       <c r="D5" s="0">
-        <v>17619.779854363675</v>
+        <v>17452.191208925429</v>
       </c>
       <c r="E5" s="0">
-        <v>5.6926765740946833e-13</v>
+        <v>1.4682544855635949e-12</v>
       </c>
       <c r="F5" s="0"/>
     </row>
@@ -18357,13 +18357,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="0">
-        <v>1.897282688866784e-12</v>
+        <v>4.7615919895931127e-12</v>
       </c>
       <c r="D6" s="0">
-        <v>17586.497240784247</v>
+        <v>17429.982104475243</v>
       </c>
       <c r="E6" s="0">
-        <v>1.897282688866784e-12</v>
+        <v>4.7615919895931127e-12</v>
       </c>
       <c r="F6" s="0"/>
     </row>
@@ -18375,13 +18375,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="0">
-        <v>6.2017400850260355e-12</v>
+        <v>1.5151308739420074e-11</v>
       </c>
       <c r="D7" s="0">
-        <v>17553.122997562044</v>
+        <v>17418.166167740423</v>
       </c>
       <c r="E7" s="0">
-        <v>6.2017400850260355e-12</v>
+        <v>1.5151308739420074e-11</v>
       </c>
       <c r="F7" s="0"/>
     </row>
@@ -18393,13 +18393,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="0">
-        <v>1.9882045386472212e-11</v>
+        <v>4.7303714339850295e-11</v>
       </c>
       <c r="D8" s="0">
-        <v>17519.588344697251</v>
+        <v>17412.369791857738</v>
       </c>
       <c r="E8" s="0">
-        <v>1.9882045386472212e-11</v>
+        <v>4.7303714339850295e-11</v>
       </c>
       <c r="F8" s="0"/>
     </row>
@@ -18411,13 +18411,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="0">
-        <v>6.2513604924729582e-11</v>
+        <v>1.4490636598147788e-10</v>
       </c>
       <c r="D9" s="0">
-        <v>17485.812041068912</v>
+        <v>17409.255823803447</v>
       </c>
       <c r="E9" s="0">
-        <v>6.2513604924729582e-11</v>
+        <v>1.4490636598147788e-10</v>
       </c>
       <c r="F9" s="0"/>
     </row>
@@ -18429,13 +18429,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="0">
-        <v>1.9277646386948166e-10</v>
+        <v>4.3553876308135763e-10</v>
       </c>
       <c r="D10" s="0">
-        <v>17451.705460906182</v>
+        <v>17409.141787819888</v>
       </c>
       <c r="E10" s="0">
-        <v>1.9277646386948166e-10</v>
+        <v>4.3553876308135763e-10</v>
       </c>
       <c r="F10" s="0"/>
     </row>
@@ -18447,13 +18447,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="0">
-        <v>5.830414870315658e-10</v>
+        <v>1.2844384210769341e-09</v>
       </c>
       <c r="D11" s="0">
-        <v>17417.175596081572</v>
+        <v>17415.920985756442</v>
       </c>
       <c r="E11" s="0">
-        <v>5.830414870315658e-10</v>
+        <v>1.2844384210769341e-09</v>
       </c>
       <c r="F11" s="0"/>
     </row>
@@ -18465,13 +18465,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="0">
-        <v>1.7294614684125718e-09</v>
+        <v>3.716609126846539e-09</v>
       </c>
       <c r="D12" s="0">
-        <v>17382.125446218815</v>
+        <v>17433.645136992549</v>
       </c>
       <c r="E12" s="0">
-        <v>1.7294614684125718e-09</v>
+        <v>3.716609126846539e-09</v>
       </c>
       <c r="F12" s="0"/>
     </row>
@@ -18483,13 +18483,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="0">
-        <v>5.0313937456560224e-09</v>
+        <v>1.0551825888609041e-08</v>
       </c>
       <c r="D13" s="0">
-        <v>17346.457091513745</v>
+        <v>17465.271558435245</v>
       </c>
       <c r="E13" s="0">
-        <v>5.0313937456560224e-09</v>
+        <v>1.0551825888609041e-08</v>
       </c>
       <c r="F13" s="0"/>
     </row>
@@ -18501,13 +18501,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="0">
-        <v>1.4355942282157667e-08</v>
+        <v>2.9393782095897528e-08</v>
       </c>
       <c r="D14" s="0">
-        <v>17310.072729833257</v>
+        <v>17507.89499176358</v>
       </c>
       <c r="E14" s="0">
-        <v>1.4355942282157667e-08</v>
+        <v>2.9393782095897528e-08</v>
       </c>
       <c r="F14" s="0"/>
     </row>
@@ -18519,13 +18519,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="0">
-        <v>4.0173630854996619e-08</v>
+        <v>8.0339745295959193e-08</v>
       </c>
       <c r="D15" s="0">
-        <v>17272.87948770171</v>
+        <v>17550.667401905008</v>
       </c>
       <c r="E15" s="0">
-        <v>4.0173630854996619e-08</v>
+        <v>8.0339745295959193e-08</v>
       </c>
       <c r="F15" s="0"/>
     </row>
@@ -18537,13 +18537,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="0">
-        <v>1.1025960916210317e-07</v>
+        <v>2.1545300571528924e-07</v>
       </c>
       <c r="D16" s="0">
-        <v>17234.805985324572</v>
+        <v>17584.622244075679</v>
       </c>
       <c r="E16" s="0">
-        <v>1.1025960916210317e-07</v>
+        <v>2.1545300571528924e-07</v>
       </c>
       <c r="F16" s="0"/>
     </row>
@@ -18555,13 +18555,13 @@
         <v>16</v>
       </c>
       <c r="C17" s="0">
-        <v>2.9679583068800667e-07</v>
+        <v>5.6692001533587895e-07</v>
       </c>
       <c r="D17" s="0">
-        <v>17195.815753468847</v>
+        <v>17608.860270752193</v>
       </c>
       <c r="E17" s="0">
-        <v>2.9679583068800667e-07</v>
+        <v>5.6692001533587895e-07</v>
       </c>
       <c r="F17" s="0"/>
     </row>
@@ -18573,13 +18573,13 @@
         <v>17</v>
       </c>
       <c r="C18" s="0">
-        <v>7.8354713307666471e-07</v>
+        <v>1.4636530754829483e-06</v>
       </c>
       <c r="D18" s="0">
-        <v>17155.914285075436</v>
+        <v>17637.255557937853</v>
       </c>
       <c r="E18" s="0">
-        <v>7.8354713307666471e-07</v>
+        <v>1.4636530754829483e-06</v>
       </c>
       <c r="F18" s="0"/>
     </row>
@@ -18591,13 +18591,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="0">
-        <v>2.0287962761288468e-06</v>
+        <v>3.7076748023526816e-06</v>
       </c>
       <c r="D19" s="0">
-        <v>17115.116198624415</v>
+        <v>17681.012097253304</v>
       </c>
       <c r="E19" s="0">
-        <v>2.0287962761288468e-06</v>
+        <v>3.7076748023526816e-06</v>
       </c>
       <c r="F19" s="0"/>
     </row>
@@ -18609,13 +18609,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="0">
-        <v>5.152022312621693e-06</v>
+        <v>9.2153587695111638e-06</v>
       </c>
       <c r="D20" s="0">
-        <v>17073.436112595857</v>
+        <v>17735.759270539285</v>
       </c>
       <c r="E20" s="0">
-        <v>5.152022312621693e-06</v>
+        <v>9.2153587695111638e-06</v>
       </c>
       <c r="F20" s="0"/>
     </row>
@@ -18627,13 +18627,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="0">
-        <v>1.2831665046542428e-05</v>
+        <v>2.24734623319022e-05</v>
       </c>
       <c r="D21" s="0">
-        <v>17030.888645469829</v>
+        <v>17785.899749970449</v>
       </c>
       <c r="E21" s="0">
-        <v>1.2831665046542428e-05</v>
+        <v>2.24734623319022e-05</v>
       </c>
       <c r="F21" s="0"/>
     </row>
@@ -18645,13 +18645,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="0">
-        <v>3.1343989749970893e-05</v>
+        <v>5.3774310605675929e-05</v>
       </c>
       <c r="D22" s="0">
-        <v>16987.488415726413</v>
+        <v>17817.409016381356</v>
       </c>
       <c r="E22" s="0">
-        <v>3.1343989749970893e-05</v>
+        <v>5.3774310605675929e-05</v>
       </c>
       <c r="F22" s="0"/>
     </row>
@@ -18663,13 +18663,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="0">
-        <v>7.5091628321427212e-05</v>
+        <v>0.00012624867906761789</v>
       </c>
       <c r="D23" s="0">
-        <v>16943.250041845677</v>
+        <v>17826.585268070405</v>
       </c>
       <c r="E23" s="0">
-        <v>7.5091628321427212e-05</v>
+        <v>0.00012624867906761789</v>
       </c>
       <c r="F23" s="0"/>
     </row>
@@ -18681,13 +18681,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="0">
-        <v>0.0001764390660053507</v>
+        <v>0.00029082113205926275</v>
       </c>
       <c r="D24" s="0">
-        <v>16898.188142307696</v>
+        <v>17815.560281943268</v>
       </c>
       <c r="E24" s="0">
-        <v>0.0001764390660053507</v>
+        <v>0.00029082113205926275</v>
       </c>
       <c r="F24" s="0"/>
     </row>
@@ -18699,13 +18699,13 @@
         <v>24</v>
       </c>
       <c r="C25" s="0">
-        <v>0.00040659680477725087</v>
+        <v>0.00065731297469422828</v>
       </c>
       <c r="D25" s="0">
-        <v>16852.317335592543</v>
+        <v>17786.010667732964</v>
       </c>
       <c r="E25" s="0">
-        <v>0.00040659680477725087</v>
+        <v>0.00065731297469422828</v>
       </c>
       <c r="F25" s="0"/>
     </row>
@@ -18717,13 +18717,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="0">
-        <v>0.00091896539088645102</v>
+        <v>0.0014576913462179622</v>
       </c>
       <c r="D26" s="0">
-        <v>16805.652240180287</v>
+        <v>17741.441923160462</v>
       </c>
       <c r="E26" s="0">
-        <v>0.00091896539088645102</v>
+        <v>0.0014576913462179622</v>
       </c>
       <c r="F26" s="0"/>
     </row>
@@ -18735,13 +18735,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="0">
-        <v>0.0020370436400632742</v>
+        <v>0.003171802028946142</v>
       </c>
       <c r="D27" s="0">
-        <v>16758.207474551004</v>
+        <v>17685.993596058841</v>
       </c>
       <c r="E27" s="0">
-        <v>0.0020370436400632742</v>
+        <v>0.003171802028946142</v>
       </c>
       <c r="F27" s="0"/>
     </row>
@@ -18753,13 +18753,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="0">
-        <v>0.0044286105821792062</v>
+        <v>0.0067716374168918375</v>
       </c>
       <c r="D28" s="0">
-        <v>16709.997657184769</v>
+        <v>17623.139197478136</v>
       </c>
       <c r="E28" s="0">
-        <v>0.0044286105821792062</v>
+        <v>0.0067716374168918375</v>
       </c>
       <c r="F28" s="0"/>
     </row>
@@ -18771,13 +18771,13 @@
         <v>28</v>
       </c>
       <c r="C29" s="0">
-        <v>0.0094427966406312978</v>
+        <v>0.014184970791775</v>
       </c>
       <c r="D29" s="0">
-        <v>16661.037406561649</v>
+        <v>17554.61254282809</v>
       </c>
       <c r="E29" s="0">
-        <v>0.0094427966406312978</v>
+        <v>0.014184970791775</v>
       </c>
       <c r="F29" s="0"/>
     </row>
@@ -18789,13 +18789,13 @@
         <v>29</v>
       </c>
       <c r="C30" s="0">
-        <v>0.019746938030262198</v>
+        <v>0.029154817158155943</v>
       </c>
       <c r="D30" s="0">
-        <v>16611.341341161726</v>
+        <v>17481.131163320119</v>
       </c>
       <c r="E30" s="0">
-        <v>0.019746938030262198</v>
+        <v>0.029154817158155943</v>
       </c>
       <c r="F30" s="0"/>
     </row>
@@ -18807,13 +18807,13 @@
         <v>30</v>
       </c>
       <c r="C31" s="0">
-        <v>0.040500918522497389</v>
+        <v>0.058794855152860828</v>
       </c>
       <c r="D31" s="0">
-        <v>16560.924079465065</v>
+        <v>17404.174813589791</v>
       </c>
       <c r="E31" s="0">
-        <v>0.040500918522497389</v>
+        <v>0.058794855152860828</v>
       </c>
       <c r="F31" s="0"/>
     </row>
@@ -18825,13 +18825,13 @@
         <v>31</v>
       </c>
       <c r="C32" s="0">
-        <v>0.081469671503673569</v>
+        <v>0.11633635534175904</v>
       </c>
       <c r="D32" s="0">
-        <v>16509.800239951739</v>
+        <v>17324.190580461935</v>
       </c>
       <c r="E32" s="0">
-        <v>0.081469671503673569</v>
+        <v>0.11633635534175904</v>
       </c>
       <c r="F32" s="0"/>
     </row>
@@ -18843,13 +18843,13 @@
         <v>32</v>
       </c>
       <c r="C33" s="0">
-        <v>0.16072855514603682</v>
+        <v>0.22585968040807233</v>
       </c>
       <c r="D33" s="0">
-        <v>16457.984441101828</v>
+        <v>17241.282602186893</v>
       </c>
       <c r="E33" s="0">
-        <v>0.16072855514603682</v>
+        <v>0.22585968040807233</v>
       </c>
       <c r="F33" s="0"/>
     </row>
@@ -18861,13 +18861,13 @@
         <v>33</v>
       </c>
       <c r="C34" s="0">
-        <v>0.31099692804863827</v>
+        <v>0.43023832206669488</v>
       </c>
       <c r="D34" s="0">
-        <v>16405.491301395399</v>
+        <v>17155.55501701502</v>
       </c>
       <c r="E34" s="0">
-        <v>0.31099692804863827</v>
+        <v>0.43023832206669488</v>
       </c>
       <c r="F34" s="0"/>
     </row>
@@ -18879,13 +18879,13 @@
         <v>34</v>
       </c>
       <c r="C35" s="0">
-        <v>0.59018088695404858</v>
+        <v>0.80413061947831654</v>
       </c>
       <c r="D35" s="0">
-        <v>16352.335439312528</v>
+        <v>17067.111963196665</v>
       </c>
       <c r="E35" s="0">
-        <v>0.59018088695404858</v>
+        <v>0.80413061947831654</v>
       </c>
       <c r="F35" s="0"/>
     </row>
@@ -18897,13 +18897,13 @@
         <v>35</v>
       </c>
       <c r="C36" s="0">
-        <v>1.0984496765382041</v>
+        <v>1.474657737979495</v>
       </c>
       <c r="D36" s="0">
-        <v>16298.531473333285</v>
+        <v>16976.057578982174</v>
       </c>
       <c r="E36" s="0">
-        <v>1.0984496765382041</v>
+        <v>1.474657737979495</v>
       </c>
       <c r="F36" s="0"/>
     </row>
@@ -18915,13 +18915,13 @@
         <v>36</v>
       </c>
       <c r="C37" s="0">
-        <v>2.0051237121919225</v>
+        <v>2.6534016514065017</v>
       </c>
       <c r="D37" s="0">
-        <v>16244.094021937746</v>
+        <v>16882.496002621901</v>
       </c>
       <c r="E37" s="0">
-        <v>2.0051237121919225</v>
+        <v>2.6534016514065017</v>
       </c>
       <c r="F37" s="0"/>
     </row>
@@ -18933,13 +18933,13 @@
         <v>37</v>
       </c>
       <c r="C38" s="0">
-        <v>3.5897827268877034</v>
+        <v>4.6844853225401781</v>
       </c>
       <c r="D38" s="0">
-        <v>16189.037703605984</v>
+        <v>16786.531372366193</v>
       </c>
       <c r="E38" s="0">
-        <v>3.5897827268877034</v>
+        <v>4.6844853225401781</v>
       </c>
       <c r="F38" s="0"/>
     </row>
@@ -18951,13 +18951,13 @@
         <v>38</v>
       </c>
       <c r="C39" s="0">
-        <v>6.3032007211771477</v>
+        <v>8.1146145697924332</v>
       </c>
       <c r="D39" s="0">
-        <v>16133.377136818068</v>
+        <v>16688.267826465399</v>
       </c>
       <c r="E39" s="0">
-        <v>6.3032007211771477</v>
+        <v>8.1146145697924332</v>
       </c>
       <c r="F39" s="0"/>
     </row>
@@ -18969,13 +18969,13 @@
         <v>39</v>
       </c>
       <c r="C40" s="0">
-        <v>10.854756706641403</v>
+        <v>13.791802731457475</v>
       </c>
       <c r="D40" s="0">
-        <v>16077.126940054075</v>
+        <v>16587.809503169872</v>
       </c>
       <c r="E40" s="0">
-        <v>10.854756706641403</v>
+        <v>13.791802731457475</v>
       </c>
       <c r="F40" s="0"/>
     </row>
@@ -18987,13 +18987,13 @@
         <v>40</v>
       </c>
       <c r="C41" s="0">
-        <v>18.333485251746765</v>
+        <v>22.999654035244202</v>
       </c>
       <c r="D41" s="0">
-        <v>16020.301731794078</v>
+        <v>16485.26054072996</v>
       </c>
       <c r="E41" s="0">
-        <v>18.333485251746765</v>
+        <v>22.999654035244202</v>
       </c>
       <c r="F41" s="0"/>
     </row>
@@ -19005,13 +19005,13 @@
         <v>41</v>
       </c>
       <c r="C42" s="0">
-        <v>30.36938213176445</v>
+        <v>37.632987515612925</v>
       </c>
       <c r="D42" s="0">
-        <v>15962.916130518146</v>
+        <v>16380.725077396011</v>
       </c>
       <c r="E42" s="0">
-        <v>30.36938213176445</v>
+        <v>37.632987515612925</v>
       </c>
       <c r="F42" s="0"/>
     </row>
@@ -19023,13 +19023,13 @@
         <v>42</v>
       </c>
       <c r="C43" s="0">
-        <v>49.339286177266992</v>
+        <v>60.417564704505068</v>
       </c>
       <c r="D43" s="0">
-        <v>15904.984754706356</v>
+        <v>16274.307251418375</v>
       </c>
       <c r="E43" s="0">
-        <v>49.339286177266992</v>
+        <v>60.417564704505068</v>
       </c>
       <c r="F43" s="0"/>
     </row>
@@ -19041,13 +19041,13 @@
         <v>43</v>
       </c>
       <c r="C44" s="0">
-        <v>78.616870296705102</v>
+        <v>95.171050201274923</v>
       </c>
       <c r="D44" s="0">
-        <v>15846.522222838781</v>
+        <v>16166.111201047403</v>
       </c>
       <c r="E44" s="0">
-        <v>78.616870296705102</v>
+        <v>95.171050201274923</v>
       </c>
       <c r="F44" s="0"/>
     </row>
@@ -19059,13 +19059,13 @@
         <v>44</v>
       </c>
       <c r="C45" s="0">
-        <v>122.85833419885219</v>
+        <v>147.09355152631534</v>
       </c>
       <c r="D45" s="0">
-        <v>15787.543153395491</v>
+        <v>16056.241064533446</v>
       </c>
       <c r="E45" s="0">
-        <v>122.85833419885219</v>
+        <v>147.09355152631534</v>
       </c>
       <c r="F45" s="0"/>
     </row>
@@ -19077,13 +19077,13 @@
         <v>45</v>
       </c>
       <c r="C46" s="0">
-        <v>188.30397045639612</v>
+        <v>223.06402410199439</v>
       </c>
       <c r="D46" s="0">
-        <v>15728.062164856561</v>
+        <v>15944.800980126849</v>
       </c>
       <c r="E46" s="0">
-        <v>188.30397045639612</v>
+        <v>223.06402410199439</v>
       </c>
       <c r="F46" s="0"/>
     </row>
@@ -19095,13 +19095,13 @@
         <v>46</v>
       </c>
       <c r="C47" s="0">
-        <v>283.06118158136854</v>
+        <v>331.90405449909861</v>
       </c>
       <c r="D47" s="0">
-        <v>15668.093875702065</v>
+        <v>15831.895086077964</v>
       </c>
       <c r="E47" s="0">
-        <v>283.06118158136854</v>
+        <v>331.90405449909861</v>
       </c>
       <c r="F47" s="0"/>
     </row>
@@ -19113,13 +19113,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="0">
-        <v>417.31801799336677</v>
+        <v>484.55458706344439</v>
       </c>
       <c r="D48" s="0">
-        <v>15607.652904412074</v>
+        <v>15717.627520637143</v>
       </c>
       <c r="E48" s="0">
-        <v>417.31801799336677</v>
+        <v>484.55458706344439</v>
       </c>
       <c r="F48" s="0"/>
     </row>
@@ -19131,13 +19131,13 @@
         <v>48</v>
       </c>
       <c r="C49" s="0">
-        <v>603.42033271563116</v>
+        <v>694.09671192981568</v>
       </c>
       <c r="D49" s="0">
-        <v>15546.753869466662</v>
+        <v>15602.102422054732</v>
       </c>
       <c r="E49" s="0">
-        <v>603.42033271563116</v>
+        <v>694.09671192981568</v>
       </c>
       <c r="F49" s="0"/>
     </row>
@@ -19149,13 +19149,13 @@
         <v>49</v>
       </c>
       <c r="C50" s="0">
-        <v>855.73388017042566</v>
+        <v>975.53844985531555</v>
       </c>
       <c r="D50" s="0">
-        <v>15485.4113893459</v>
+        <v>15485.423928581082</v>
       </c>
       <c r="E50" s="0">
-        <v>855.73388017042566</v>
+        <v>975.53844985531555</v>
       </c>
       <c r="F50" s="0"/>
     </row>
@@ -19167,13 +19167,13 @@
         <v>50</v>
       </c>
       <c r="C51" s="0">
-        <v>1190.2097314372979</v>
+        <v>1345.2900249962574</v>
       </c>
       <c r="D51" s="0">
-        <v>15423.640082529864</v>
+        <v>15367.696178466542</v>
       </c>
       <c r="E51" s="0">
-        <v>1190.2097314372979</v>
+        <v>1345.2900249962574</v>
       </c>
       <c r="F51" s="0"/>
     </row>
@@ -19185,13 +19185,13 @@
         <v>51</v>
       </c>
       <c r="C52" s="0">
-        <v>1623.5820821840871</v>
+        <v>1820.264834545193</v>
       </c>
       <c r="D52" s="0">
-        <v>15361.454567498626</v>
+        <v>15249.023309961463</v>
       </c>
       <c r="E52" s="0">
-        <v>1623.5820821840871</v>
+        <v>1820.264834545193</v>
       </c>
       <c r="F52" s="0"/>
     </row>
@@ -19203,13 +19203,13 @@
         <v>52</v>
       </c>
       <c r="C53" s="0">
-        <v>2172.155867877229</v>
+        <v>2416.5754688989832</v>
       </c>
       <c r="D53" s="0">
-        <v>15298.869462732258</v>
+        <v>15129.509461316193</v>
       </c>
       <c r="E53" s="0">
-        <v>2172.155867877229</v>
+        <v>2416.5754688989832</v>
       </c>
       <c r="F53" s="0"/>
     </row>
@@ -19221,13 +19221,13 @@
         <v>53</v>
       </c>
       <c r="C54" s="0">
-        <v>2850.1892965484521</v>
+        <v>3147.8445137037461</v>
       </c>
       <c r="D54" s="0">
-        <v>15235.899386710833</v>
+        <v>15009.258770781082</v>
       </c>
       <c r="E54" s="0">
-        <v>2850.1892965484521</v>
+        <v>3147.8445137037461</v>
       </c>
       <c r="F54" s="0"/>
     </row>
@@ -19239,13 +19239,13 @@
         <v>54</v>
       </c>
       <c r="C55" s="0">
-        <v>3667.9415538448548</v>
+        <v>4023.2156197623763</v>
       </c>
       <c r="D55" s="0">
-        <v>15172.558957914425</v>
+        <v>14888.375376606482</v>
       </c>
       <c r="E55" s="0">
-        <v>3667.9415538448548</v>
+        <v>4023.2156197623763</v>
       </c>
       <c r="F55" s="0"/>
     </row>
@@ -19257,13 +19257,13 @@
         <v>55</v>
       </c>
       <c r="C56" s="0">
-        <v>4629.5320168948838</v>
+        <v>5045.2242138959673</v>
       </c>
       <c r="D56" s="0">
-        <v>15108.862794823108</v>
+        <v>14766.963417042738</v>
       </c>
       <c r="E56" s="0">
-        <v>4629.5320168948838</v>
+        <v>5045.2242138959673</v>
       </c>
       <c r="F56" s="0"/>
     </row>
@@ -19275,13 +19275,13 @@
         <v>56</v>
       </c>
       <c r="C57" s="0">
-        <v>5730.8330923214144</v>
+        <v>6207.7577457817079</v>
       </c>
       <c r="D57" s="0">
-        <v>15044.825515916953</v>
+        <v>14645.127030340205</v>
       </c>
       <c r="E57" s="0">
-        <v>5730.8330923214144</v>
+        <v>6207.7577457817079</v>
       </c>
       <c r="F57" s="0"/>
     </row>
@@ -19293,13 +19293,13 @@
         <v>57</v>
       </c>
       <c r="C58" s="0">
-        <v>6957.6793671729638</v>
+        <v>7494.3880397348439</v>
       </c>
       <c r="D58" s="0">
-        <v>14980.461739676033</v>
+        <v>14522.970354749228</v>
       </c>
       <c r="E58" s="0">
-        <v>6957.6793671729638</v>
+        <v>7494.3880397348439</v>
       </c>
       <c r="F58" s="0"/>
     </row>
@@ -19311,13 +19311,13 @@
         <v>58</v>
       </c>
       <c r="C59" s="0">
-        <v>8284.7049337794906</v>
+        <v>8877.3781074709059</v>
       </c>
       <c r="D59" s="0">
-        <v>14915.786084580423</v>
+        <v>14400.597528520158</v>
       </c>
       <c r="E59" s="0">
-        <v>8284.7049337794906</v>
+        <v>8877.3781074709059</v>
       </c>
       <c r="F59" s="0"/>
     </row>
@@ -19329,13 +19329,13 @@
         <v>59</v>
       </c>
       <c r="C60" s="0">
-        <v>9675.1044547628899</v>
+        <v>10317.640370794474</v>
       </c>
       <c r="D60" s="0">
-        <v>14850.813169110192</v>
+        <v>14278.112689903346</v>
       </c>
       <c r="E60" s="0">
-        <v>9675.1044547628899</v>
+        <v>10317.640370794474</v>
       </c>
       <c r="F60" s="0"/>
     </row>
@@ -19347,13 +19347,13 @@
         <v>60</v>
       </c>
       <c r="C61" s="0">
-        <v>11081.543680246703</v>
+        <v>11765.846571581575</v>
       </c>
       <c r="D61" s="0">
-        <v>14785.557611745418</v>
+        <v>14155.619977149141</v>
       </c>
       <c r="E61" s="0">
-        <v>11081.543680246703</v>
+        <v>11765.846571581575</v>
       </c>
       <c r="F61" s="0"/>
     </row>
@@ -19365,13 +19365,13 @@
         <v>61</v>
       </c>
       <c r="C62" s="0">
-        <v>12448.322923499809</v>
+        <v>13164.764722645878</v>
       </c>
       <c r="D62" s="0">
-        <v>14720.034030966171</v>
+        <v>14033.223528507891</v>
       </c>
       <c r="E62" s="0">
-        <v>12448.322923499809</v>
+        <v>13164.764722645878</v>
       </c>
       <c r="F62" s="0"/>
     </row>
@@ -19383,13 +19383,13 @@
         <v>62</v>
       </c>
       <c r="C63" s="0">
-        <v>13714.734736745302</v>
+        <v>14452.738651001438</v>
       </c>
       <c r="D63" s="0">
-        <v>14654.257045252523</v>
+        <v>13911.027482229947</v>
       </c>
       <c r="E63" s="0">
-        <v>13714.734736745302</v>
+        <v>14452.738651001438</v>
       </c>
       <c r="F63" s="0"/>
     </row>
@@ -19401,13 +19401,13 @@
         <v>63</v>
       </c>
       <c r="C64" s="0">
-        <v>14819.377508891208</v>
+        <v>15568.053783115707</v>
       </c>
       <c r="D64" s="0">
-        <v>14588.24127308455</v>
+        <v>13789.135976565658</v>
       </c>
       <c r="E64" s="0">
-        <v>14819.377508891208</v>
+        <v>15568.053783115707</v>
       </c>
       <c r="F64" s="0"/>
     </row>
@@ -19419,13 +19419,13 @@
         <v>64</v>
       </c>
       <c r="C65" s="0">
-        <v>15705.019996020061</v>
+        <v>16453.777629455577</v>
       </c>
       <c r="D65" s="0">
-        <v>14522.001332942324</v>
+        <v>13667.653149765376</v>
       </c>
       <c r="E65" s="0">
-        <v>15705.019996020061</v>
+        <v>16453.777629455577</v>
       </c>
       <c r="F65" s="0"/>
     </row>
@@ -19437,13 +19437,13 @@
         <v>65</v>
       </c>
       <c r="C66" s="0">
-        <v>16323.489680413761</v>
+        <v>17062.554448621224</v>
       </c>
       <c r="D66" s="0">
-        <v>14455.551843305917</v>
+        <v>13546.683140079447</v>
       </c>
       <c r="E66" s="0">
-        <v>16323.489680413761</v>
+        <v>17062.554448621224</v>
       </c>
       <c r="F66" s="0"/>
     </row>
@@ -19455,13 +19455,13 @@
         <v>66</v>
       </c>
       <c r="C67" s="0">
-        <v>16640.007103609212</v>
+        <v>17360.794779922493</v>
       </c>
       <c r="D67" s="0">
-        <v>14388.907422655404</v>
+        <v>13426.330085758222</v>
       </c>
       <c r="E67" s="0">
-        <v>16640.007103609212</v>
+        <v>17360.794779922493</v>
       </c>
       <c r="F67" s="0"/>
     </row>
@@ -19473,13 +19473,13 @@
         <v>67</v>
       </c>
       <c r="C68" s="0">
-        <v>16623.884810448581</v>
+        <v>17331.74468777686</v>
       </c>
       <c r="D68" s="0">
-        <v>14322.082689470853</v>
+        <v>13306.698125052051</v>
       </c>
       <c r="E68" s="0">
-        <v>16623.884810448581</v>
+        <v>17331.74468777686</v>
       </c>
       <c r="F68" s="0"/>
     </row>
@@ -19491,13 +19491,13 @@
         <v>68</v>
       </c>
       <c r="C69" s="0">
-        <v>16205.777838251204</v>
+        <v>16977.044567742229</v>
       </c>
       <c r="D69" s="0">
-        <v>14255.092262232343</v>
+        <v>13187.891396211284</v>
       </c>
       <c r="E69" s="0">
-        <v>16205.777838251204</v>
+        <v>16977.044567742229</v>
       </c>
       <c r="F69" s="0"/>
     </row>
@@ -19509,13 +19509,13 @@
         <v>69</v>
       </c>
       <c r="C70" s="0">
-        <v>15405.149641158563</v>
+        <v>16316.575732526444</v>
       </c>
       <c r="D70" s="0">
-        <v>14187.950759419946</v>
+        <v>13070.014037486269</v>
       </c>
       <c r="E70" s="0">
-        <v>15405.149641158563</v>
+        <v>16316.575732526444</v>
       </c>
       <c r="F70" s="0"/>
     </row>
@@ -19527,13 +19527,13 @@
         <v>70</v>
       </c>
       <c r="C71" s="0">
-        <v>14279.751240665626</v>
+        <v>15386.614739156619</v>
       </c>
       <c r="D71" s="0">
-        <v>14120.67279951373</v>
+        <v>12953.170187127358</v>
       </c>
       <c r="E71" s="0">
-        <v>14279.751240665626</v>
+        <v>15386.614739156619</v>
       </c>
       <c r="F71" s="0"/>
     </row>
@@ -19545,13 +19545,13 @@
         <v>71</v>
       </c>
       <c r="C72" s="0">
-        <v>12907.259536274121</v>
+        <v>14236.533842856976</v>
       </c>
       <c r="D72" s="0">
-        <v>14053.273000993773</v>
+        <v>12837.4639833849</v>
       </c>
       <c r="E72" s="0">
-        <v>12907.259536274121</v>
+        <v>14236.533842856976</v>
       </c>
       <c r="F72" s="0"/>
     </row>
@@ -19563,13 +19563,13 @@
         <v>72</v>
       </c>
       <c r="C73" s="0">
-        <v>11376.43327824757</v>
+        <v>12924.46504636696</v>
       </c>
       <c r="D73" s="0">
-        <v>13985.765982340148</v>
+        <v>12722.999564509242</v>
       </c>
       <c r="E73" s="0">
-        <v>11376.43327824757</v>
+        <v>12924.46504636696</v>
       </c>
       <c r="F73" s="0"/>
     </row>
@@ -19581,13 +19581,13 @@
         <v>73</v>
       </c>
       <c r="C74" s="0">
-        <v>9777.703996439277</v>
+        <v>11512.456819035282</v>
       </c>
       <c r="D74" s="0">
-        <v>13918.166362032924</v>
+        <v>12609.881068750734</v>
       </c>
       <c r="E74" s="0">
-        <v>9777.703996439277</v>
+        <v>11512.456819035282</v>
       </c>
       <c r="F74" s="0"/>
     </row>
@@ -19599,13 +19599,13 @@
         <v>74</v>
       </c>
       <c r="C75" s="0">
-        <v>8194.5729809119603</v>
+        <v>10061.681797322464</v>
       </c>
       <c r="D75" s="0">
-        <v>13850.488758552177</v>
+        <v>12498.21263435973</v>
       </c>
       <c r="E75" s="0">
-        <v>8194.5729809119603</v>
+        <v>10061.681797322464</v>
       </c>
       <c r="F75" s="0"/>
     </row>
@@ -19617,13 +19617,13 @@
         <v>75</v>
       </c>
       <c r="C76" s="0">
-        <v>6696.90980052945</v>
+        <v>8628.2013083252896</v>
       </c>
       <c r="D76" s="0">
-        <v>13782.747790377982</v>
+        <v>12388.098399586575</v>
       </c>
       <c r="E76" s="0">
-        <v>6696.90980052945</v>
+        <v>8628.2013083252896</v>
       </c>
       <c r="F76" s="0"/>
     </row>
@@ -19635,13 +19635,13 @@
         <v>76</v>
       </c>
       <c r="C77" s="0">
-        <v>5336.8039854049957</v>
+        <v>7259.6734564564749</v>
       </c>
       <c r="D77" s="0">
-        <v>13714.958075990407</v>
+        <v>12279.642502681621</v>
       </c>
       <c r="E77" s="0">
-        <v>5336.8039854049957</v>
+        <v>7259.6734564564749</v>
       </c>
       <c r="F77" s="0"/>
     </row>
@@ -19653,13 +19653,13 @@
         <v>77</v>
       </c>
       <c r="C78" s="0">
-        <v>4147.1212653553921</v>
+        <v>5993.2311743494229</v>
       </c>
       <c r="D78" s="0">
-        <v>13647.134233869529</v>
+        <v>12172.949081895214</v>
       </c>
       <c r="E78" s="0">
-        <v>4147.1212653553921</v>
+        <v>5993.2311743494229</v>
       </c>
       <c r="F78" s="0"/>
     </row>
@@ -19671,13 +19671,13 @@
         <v>78</v>
       </c>
       <c r="C79" s="0">
-        <v>3142.4682444829855</v>
+        <v>4854.584889734153</v>
       </c>
       <c r="D79" s="0">
-        <v>13579.290882495417</v>
+        <v>12068.12227547771</v>
       </c>
       <c r="E79" s="0">
-        <v>3142.4682444829855</v>
+        <v>4854.584889734153</v>
       </c>
       <c r="F79" s="0"/>
     </row>
@@ -19689,13 +19689,13 @@
         <v>79</v>
       </c>
       <c r="C80" s="0">
-        <v>2321.9546913742279</v>
+        <v>3858.2493890901919</v>
       </c>
       <c r="D80" s="0">
-        <v>13511.442640348148</v>
+        <v>11965.266221679454</v>
       </c>
       <c r="E80" s="0">
-        <v>2321.9546913742279</v>
+        <v>3858.2493890901919</v>
       </c>
       <c r="F80" s="0"/>
     </row>
@@ -19707,13 +19707,13 @@
         <v>80</v>
       </c>
       <c r="C81" s="0">
-        <v>1672.9973947289666</v>
+        <v>3008.6773654217995</v>
       </c>
       <c r="D81" s="0">
-        <v>13443.604125907794</v>
+        <v>11864.485058750797</v>
       </c>
       <c r="E81" s="0">
-        <v>1672.9973947289666</v>
+        <v>3008.6773654217995</v>
       </c>
       <c r="F81" s="0"/>
     </row>
@@ -19725,13 +19725,13 @@
         <v>81</v>
       </c>
       <c r="C82" s="0">
-        <v>1175.426475423528</v>
+        <v>2302.0145692560955</v>
       </c>
       <c r="D82" s="0">
-        <v>13375.789957654428</v>
+        <v>11765.882924942089</v>
       </c>
       <c r="E82" s="0">
-        <v>1175.426475423528</v>
+        <v>2302.0145692560955</v>
       </c>
       <c r="F82" s="0"/>
     </row>
@@ -19743,13 +19743,13 @@
         <v>82</v>
       </c>
       <c r="C83" s="0">
-        <v>805.29379509275111</v>
+        <v>1728.174702125538</v>
       </c>
       <c r="D83" s="0">
-        <v>13308.014754068121</v>
+        <v>11669.563958503677</v>
       </c>
       <c r="E83" s="0">
-        <v>805.29379509275111</v>
+        <v>1728.174702125538</v>
       </c>
       <c r="F83" s="0"/>
     </row>
@@ -19761,13 +19761,13 @@
         <v>83</v>
       </c>
       <c r="C84" s="0">
-        <v>537.98716833322032</v>
+        <v>1272.958793076031</v>
       </c>
       <c r="D84" s="0">
-        <v>13240.293133628948</v>
+        <v>11575.632297685912</v>
       </c>
       <c r="E84" s="0">
-        <v>537.98716833322032</v>
+        <v>1272.958793076031</v>
       </c>
       <c r="F84" s="0"/>
     </row>
@@ -19779,13 +19779,13 @@
         <v>84</v>
       </c>
       <c r="C85" s="0">
-        <v>350.46783209292192</v>
+        <v>920.0007336224503</v>
       </c>
       <c r="D85" s="0">
-        <v>13172.63971481698</v>
+        <v>11484.192080739145</v>
       </c>
       <c r="E85" s="0">
-        <v>350.46783209292192</v>
+        <v>920.0007336224503</v>
       </c>
       <c r="F85" s="0"/>
     </row>
@@ -19797,13 +19797,13 @@
         <v>85</v>
       </c>
       <c r="C86" s="0">
-        <v>222.62969291520901</v>
+        <v>652.39275340684867</v>
       </c>
       <c r="D86" s="0">
-        <v>13105.069116112292</v>
+        <v>11395.347445913725</v>
       </c>
       <c r="E86" s="0">
-        <v>222.62969291520901</v>
+        <v>652.39275340684867</v>
       </c>
       <c r="F86" s="0"/>
     </row>
@@ -19815,13 +19815,13 @@
         <v>86</v>
       </c>
       <c r="C87" s="0">
-        <v>137.90394580169826</v>
+        <v>453.91779574441819</v>
       </c>
       <c r="D87" s="0">
-        <v>13037.595955994959</v>
+        <v>11309.20253146</v>
       </c>
       <c r="E87" s="0">
-        <v>137.90394580169826</v>
+        <v>453.91779574441819</v>
       </c>
       <c r="F87" s="0"/>
     </row>
@@ -19833,13 +19833,13 @@
         <v>87</v>
       </c>
       <c r="C88" s="0">
-        <v>83.296926758912264</v>
+        <v>309.87919351651107</v>
       </c>
       <c r="D88" s="0">
-        <v>12970.23485294505</v>
+        <v>11225.861475628322</v>
       </c>
       <c r="E88" s="0">
-        <v>83.296926758912264</v>
+        <v>309.87919351651107</v>
       </c>
       <c r="F88" s="0"/>
     </row>
@@ -19851,13 +19851,13 @@
         <v>88</v>
       </c>
       <c r="C89" s="0">
-        <v>49.061400846013612</v>
+        <v>207.56529973023527</v>
       </c>
       <c r="D89" s="0">
-        <v>12903.000425442637</v>
+        <v>11145.42841666904</v>
       </c>
       <c r="E89" s="0">
-        <v>49.061400846013612</v>
+        <v>207.56529973023527</v>
       </c>
       <c r="F89" s="0"/>
     </row>
@@ -19869,13 +19869,13 @@
         <v>89</v>
       </c>
       <c r="C90" s="0">
-        <v>28.177962754157189</v>
+        <v>136.41565457044038</v>
       </c>
       <c r="D90" s="0">
-        <v>12835.907291967798</v>
+        <v>11068.007492832501</v>
       </c>
       <c r="E90" s="0">
-        <v>28.177962754157189</v>
+        <v>136.41565457044038</v>
       </c>
       <c r="F90" s="0"/>
     </row>
@@ -19887,13 +19887,13 @@
         <v>90</v>
       </c>
       <c r="C91" s="0">
-        <v>15.781123456662339</v>
+        <v>87.967205955061758</v>
       </c>
       <c r="D91" s="0">
-        <v>12768.970071000602</v>
+        <v>10993.702842369059</v>
       </c>
       <c r="E91" s="0">
-        <v>15.781123456662339</v>
+        <v>87.967205955061758</v>
       </c>
       <c r="F91" s="0"/>
     </row>
@@ -19905,13 +19905,13 @@
         <v>91</v>
       </c>
       <c r="C92" s="0">
-        <v>8.6183658164697032</v>
+        <v>55.657604591035735</v>
       </c>
       <c r="D92" s="0">
-        <v>12702.203381021125</v>
+        <v>10922.618603529059</v>
       </c>
       <c r="E92" s="0">
-        <v>8.6183658164697032</v>
+        <v>55.657604591035735</v>
       </c>
       <c r="F92" s="0"/>
     </row>
@@ -19923,13 +19923,13 @@
         <v>92</v>
       </c>
       <c r="C93" s="0">
-        <v>4.5895553465883641</v>
+        <v>34.552171814896113</v>
       </c>
       <c r="D93" s="0">
-        <v>12635.621840509437</v>
+        <v>10854.858914562854</v>
       </c>
       <c r="E93" s="0">
-        <v>4.5895553465883641</v>
+        <v>34.552171814896113</v>
       </c>
       <c r="F93" s="0"/>
     </row>
@@ -19941,13 +19941,13 @@
         <v>93</v>
       </c>
       <c r="C94" s="0">
-        <v>2.383279508911663</v>
+        <v>21.046181750369147</v>
       </c>
       <c r="D94" s="0">
-        <v>12569.240067945611</v>
+        <v>10790.527913720794</v>
       </c>
       <c r="E94" s="0">
-        <v>2.383279508911663</v>
+        <v>21.046181750369147</v>
       </c>
       <c r="F94" s="0"/>
     </row>
@@ -19959,13 +19959,13 @@
         <v>94</v>
       </c>
       <c r="C95" s="0">
-        <v>1.2068075730288887</v>
+        <v>12.578197478051436</v>
       </c>
       <c r="D95" s="0">
-        <v>12503.072681809725</v>
+        <v>10729.729739253225</v>
       </c>
       <c r="E95" s="0">
-        <v>1.2068075730288887</v>
+        <v>12.578197478051436</v>
       </c>
       <c r="F95" s="0"/>
     </row>
@@ -19977,13 +19977,13 @@
         <v>95</v>
       </c>
       <c r="C96" s="0">
-        <v>0.59588129775790022</v>
+        <v>7.3758254005187709</v>
       </c>
       <c r="D96" s="0">
-        <v>12437.134300581845</v>
+        <v>10672.568529410499</v>
       </c>
       <c r="E96" s="0">
-        <v>0.59588129775790022</v>
+        <v>7.3758254005187709</v>
       </c>
       <c r="F96" s="0"/>
     </row>
@@ -19995,13 +19995,13 @@
         <v>96</v>
       </c>
       <c r="C97" s="0">
-        <v>0.28690635192079361</v>
+        <v>4.2437517697946676</v>
       </c>
       <c r="D97" s="0">
-        <v>12371.43954274205</v>
+        <v>10619.148422442966</v>
       </c>
       <c r="E97" s="0">
-        <v>0.28690635192079361</v>
+        <v>4.2437517697946676</v>
       </c>
       <c r="F97" s="0"/>
     </row>
@@ -20013,13 +20013,13 @@
         <v>97</v>
       </c>
       <c r="C98" s="0">
-        <v>0.13470361535870842</v>
+        <v>2.3957221281939391</v>
       </c>
       <c r="D98" s="0">
-        <v>12306.003026770408</v>
+        <v>10569.573556600975</v>
       </c>
       <c r="E98" s="0">
-        <v>0.13470361535870842</v>
+        <v>2.3957221281939391</v>
       </c>
       <c r="F98" s="0"/>
     </row>
@@ -20031,13 +20031,13 @@
         <v>98</v>
       </c>
       <c r="C99" s="0">
-        <v>0.061670436319453771</v>
+        <v>1.3269973091207701</v>
       </c>
       <c r="D99" s="0">
-        <v>12240.839371146994</v>
+        <v>10523.948070134873</v>
       </c>
       <c r="E99" s="0">
-        <v>0.061670436319453771</v>
+        <v>1.3269973091207701</v>
       </c>
       <c r="F99" s="0"/>
     </row>
@@ -20049,13 +20049,13 @@
         <v>99</v>
       </c>
       <c r="C100" s="0">
-        <v>0.027531728006693762</v>
+        <v>0.72119177744612761</v>
       </c>
       <c r="D100" s="0">
-        <v>12175.963194351883</v>
+        <v>10482.376101295016</v>
       </c>
       <c r="E100" s="0">
-        <v>0.027531728006693762</v>
+        <v>0.72119177744612761</v>
       </c>
       <c r="F100" s="0"/>
     </row>
@@ -20067,13 +20067,13 @@
         <v>100</v>
       </c>
       <c r="C101" s="0">
-        <v>0.011985291467500499</v>
+        <v>0.38457284692500954</v>
       </c>
       <c r="D101" s="0">
-        <v>12111.389114865147</v>
+        <v>10444.961788331744</v>
       </c>
       <c r="E101" s="0">
-        <v>0.011985291467500499</v>
+        <v>0.38457284692500954</v>
       </c>
       <c r="F101" s="0"/>
     </row>
@@ -20085,13 +20085,13 @@
         <v>101</v>
       </c>
       <c r="C102" s="0">
-        <v>0.0050877107193049529</v>
+        <v>0.20121186867240606</v>
       </c>
       <c r="D102" s="0">
-        <v>12047.131751166857</v>
+        <v>10411.809269495418</v>
       </c>
       <c r="E102" s="0">
-        <v>0.0050877107193049529</v>
+        <v>0.20121186867240606</v>
       </c>
       <c r="F102" s="0"/>
     </row>
@@ -20103,13 +20103,13 @@
         <v>102</v>
       </c>
       <c r="C103" s="0">
-        <v>0.0021059831890861518</v>
+        <v>0.10329414327613305</v>
       </c>
       <c r="D103" s="0">
-        <v>11983.205721737088</v>
+        <v>10383.022683036379</v>
       </c>
       <c r="E103" s="0">
-        <v>0.0021059831890861518</v>
+        <v>0.10329414327613305</v>
       </c>
       <c r="F103" s="0"/>
     </row>
@@ -20121,13 +20121,13 @@
         <v>103</v>
       </c>
       <c r="C104" s="0">
-        <v>0.00085005312963378193</v>
+        <v>0.052028933998229027</v>
       </c>
       <c r="D104" s="0">
-        <v>11919.625645055912</v>
+        <v>10358.70616720498</v>
       </c>
       <c r="E104" s="0">
-        <v>0.00085005312963378193</v>
+        <v>0.052028933998229027</v>
       </c>
       <c r="F104" s="0"/>
     </row>
@@ -20139,13 +20139,13 @@
         <v>104</v>
       </c>
       <c r="C105" s="0">
-        <v>0.00033457687575672246</v>
+        <v>0.025713505296083673</v>
       </c>
       <c r="D105" s="0">
-        <v>11856.406139603401</v>
+        <v>10338.96386025157</v>
       </c>
       <c r="E105" s="0">
-        <v>0.00033457687575672246</v>
+        <v>0.025713505296083673</v>
       </c>
       <c r="F105" s="0"/>
     </row>
@@ -20157,13 +20157,13 @@
         <v>105</v>
       </c>
       <c r="C106" s="0">
-        <v>0.00012841165773763485</v>
+        <v>0.012468803102820484</v>
       </c>
       <c r="D106" s="0">
-        <v>11793.561823859631</v>
+        <v>10323.899900426499</v>
       </c>
       <c r="E106" s="0">
-        <v>0.00012841165773763485</v>
+        <v>0.012468803102820484</v>
       </c>
       <c r="F106" s="0"/>
     </row>
@@ -20175,13 +20175,13 @@
         <v>106</v>
       </c>
       <c r="C107" s="0">
-        <v>4.8058660729000036e-05</v>
+        <v>0.0059324676150424643</v>
       </c>
       <c r="D107" s="0">
-        <v>11731.107316304671</v>
+        <v>10313.618425980118</v>
       </c>
       <c r="E107" s="0">
-        <v>4.8058660729000036e-05</v>
+        <v>0.0059324676150424643</v>
       </c>
       <c r="F107" s="0"/>
     </row>
@@ -20193,13 +20193,13 @@
         <v>107</v>
       </c>
       <c r="C108" s="0">
-        <v>1.753870630574165e-05</v>
+        <v>0.0027694473402492528</v>
       </c>
       <c r="D108" s="0">
-        <v>11669.057235418599</v>
+        <v>10308.223575162772</v>
       </c>
       <c r="E108" s="0">
-        <v>1.753870630574165e-05</v>
+        <v>0.0027694473402492528</v>
       </c>
       <c r="F108" s="0"/>
     </row>
@@ -20211,13 +20211,13 @@
         <v>108</v>
       </c>
       <c r="C109" s="0">
-        <v>6.2414015962013367e-06</v>
+        <v>0.0012685219123700247</v>
       </c>
       <c r="D109" s="0">
-        <v>11607.426199681484</v>
+        <v>10307.819486224815</v>
       </c>
       <c r="E109" s="0">
-        <v>6.2414015962013367e-06</v>
+        <v>0.0012685219123700247</v>
       </c>
       <c r="F109" s="0"/>
     </row>
@@ -20229,13 +20229,13 @@
         <v>109</v>
       </c>
       <c r="C110" s="0">
-        <v>2.1658350615391573e-06</v>
+        <v>0.00057009858351680074</v>
       </c>
       <c r="D110" s="0">
-        <v>11546.228827573399</v>
+        <v>10312.510297416595</v>
       </c>
       <c r="E110" s="0">
-        <v>2.1658350615391573e-06</v>
+        <v>0.00057009858351680074</v>
       </c>
       <c r="F110" s="0"/>
     </row>
@@ -20247,13 +20247,13 @@
         <v>110</v>
       </c>
       <c r="C111" s="0">
-        <v>7.3287062162253062e-07</v>
+        <v>0.0002513906244173975</v>
       </c>
       <c r="D111" s="0">
-        <v>11485.47973757442</v>
+        <v>10322.400146988461</v>
       </c>
       <c r="E111" s="0">
-        <v>7.3287062162253062e-07</v>
+        <v>0.0002513906244173975</v>
       </c>
       <c r="F111" s="0"/>
     </row>
@@ -20265,13 +20265,13 @@
         <v>111</v>
       </c>
       <c r="C112" s="0">
-        <v>2.4181761055502992e-07</v>
+        <v>0.00010876654113711836</v>
       </c>
       <c r="D112" s="0">
-        <v>11425.193548164618</v>
+        <v>10337.593173190764</v>
       </c>
       <c r="E112" s="0">
-        <v>2.4181761055502992e-07</v>
+        <v>0.00010876654113711836</v>
       </c>
       <c r="F112" s="0"/>
     </row>
@@ -20283,13 +20283,13 @@
         <v>112</v>
       </c>
       <c r="C113" s="0">
-        <v>7.7804948344259691e-08</v>
+        <v>4.6173062992143335e-05</v>
       </c>
       <c r="D113" s="0">
-        <v>11365.384877824066</v>
+        <v>10358.193514273851</v>
       </c>
       <c r="E113" s="0">
-        <v>7.7804948344259691e-08</v>
+        <v>4.6173062992143335e-05</v>
       </c>
       <c r="F113" s="0"/>
     </row>
@@ -20301,13 +20301,13 @@
         <v>113</v>
       </c>
       <c r="C114" s="0">
-        <v>2.4410978725479321e-08</v>
+        <v>1.9232209417788576e-05</v>
       </c>
       <c r="D114" s="0">
-        <v>11306.068345032836</v>
+        <v>10384.305308488076</v>
       </c>
       <c r="E114" s="0">
-        <v>2.4410978725479321e-08</v>
+        <v>1.9232209417788576e-05</v>
       </c>
       <c r="F114" s="0"/>
     </row>
@@ -20319,13 +20319,13 @@
         <v>114</v>
       </c>
       <c r="C115" s="0">
-        <v>7.4683015628770668e-09</v>
+        <v>7.8598960014957854e-06</v>
       </c>
       <c r="D115" s="0">
-        <v>11247.258568271005</v>
+        <v>10416.032694083786</v>
       </c>
       <c r="E115" s="0">
-        <v>7.4683015628770668e-09</v>
+        <v>7.8598960014957854e-06</v>
       </c>
       <c r="F115" s="0"/>
     </row>
@@ -20337,13 +20337,13 @@
         <v>115</v>
       </c>
       <c r="C116" s="0">
-        <v>2.2280102276657704e-09</v>
+        <v>3.151748439284262e-06</v>
       </c>
       <c r="D116" s="0">
-        <v>11188.97016601864</v>
+        <v>10452.808944053284</v>
       </c>
       <c r="E116" s="0">
-        <v>2.2280102276657704e-09</v>
+        <v>3.151748439284262e-06</v>
       </c>
       <c r="F116" s="0"/>
     </row>
@@ -20355,13 +20355,13 @@
         <v>116</v>
       </c>
       <c r="C117" s="0">
-        <v>6.4814353661228826e-10</v>
+        <v>1.2400335046899884e-06</v>
       </c>
       <c r="D117" s="0">
-        <v>11131.217756755821</v>
+        <v>10490.200564869792</v>
       </c>
       <c r="E117" s="0">
-        <v>6.4814353661228826e-10</v>
+        <v>1.2400335046899884e-06</v>
       </c>
       <c r="F117" s="0"/>
     </row>
@@ -20373,13 +20373,13 @@
         <v>117</v>
       </c>
       <c r="C118" s="0">
-        <v>1.8385857476974273e-10</v>
+        <v>4.7869888857872579e-07</v>
       </c>
       <c r="D118" s="0">
-        <v>11074.015958962613</v>
+        <v>10518.399705528327</v>
       </c>
       <c r="E118" s="0">
-        <v>1.8385857476974273e-10</v>
+        <v>4.7869888857872579e-07</v>
       </c>
       <c r="F118" s="0"/>
     </row>
@@ -20391,13 +20391,13 @@
         <v>118</v>
       </c>
       <c r="C119" s="0">
-        <v>5.0857530034254488e-11</v>
+        <v>1.8131700848991661e-07</v>
       </c>
       <c r="D119" s="0">
-        <v>11017.379391119095</v>
+        <v>10526.57896529834</v>
       </c>
       <c r="E119" s="0">
-        <v>5.0857530034254488e-11</v>
+        <v>1.8131700848991661e-07</v>
       </c>
       <c r="F119" s="0"/>
     </row>
@@ -20409,13 +20409,13 @@
         <v>119</v>
       </c>
       <c r="C120" s="0">
-        <v>1.3717826937459153e-11</v>
+        <v>6.7384777310436479e-08</v>
       </c>
       <c r="D120" s="0">
-        <v>10961.322671705339</v>
+        <v>10505.807751187578</v>
       </c>
       <c r="E120" s="0">
-        <v>1.3717826937459153e-11</v>
+        <v>6.7384777310436479e-08</v>
       </c>
       <c r="F120" s="0"/>
     </row>
@@ -20427,13 +20427,13 @@
         <v>120</v>
       </c>
       <c r="C121" s="0">
-        <v>3.6080625268215613e-12</v>
+        <v>2.457152867698945e-08</v>
       </c>
       <c r="D121" s="0">
-        <v>10905.860419201415</v>
+        <v>10456.772368407239</v>
       </c>
       <c r="E121" s="0">
-        <v>3.6080625268215613e-12</v>
+        <v>2.457152867698945e-08</v>
       </c>
       <c r="F121" s="0"/>
     </row>
@@ -20445,13 +20445,13 @@
         <v>121</v>
       </c>
       <c r="C122" s="0">
-        <v>9.2538290228206055e-13</v>
+        <v>8.7912307892321713e-09</v>
       </c>
       <c r="D122" s="0">
-        <v>10851.007252087402</v>
+        <v>10393.453202689096</v>
       </c>
       <c r="E122" s="0">
-        <v>9.2538290228206055e-13</v>
+        <v>8.7912307892321713e-09</v>
       </c>
       <c r="F122" s="0"/>
     </row>
@@ -20463,13 +20463,13 @@
         <v>122</v>
       </c>
       <c r="C123" s="0">
-        <v>2.3143421619094569e-13</v>
+        <v>3.086130686747692e-09</v>
       </c>
       <c r="D123" s="0">
-        <v>10796.777788843365</v>
+        <v>10332.55190050487</v>
       </c>
       <c r="E123" s="0">
-        <v>2.3143421619094569e-13</v>
+        <v>3.086130686747692e-09</v>
       </c>
       <c r="F123" s="0"/>
     </row>
@@ -20481,13 +20481,13 @@
         <v>123</v>
       </c>
       <c r="C124" s="0">
-        <v>5.6440693806919969e-14</v>
+        <v>1.0629823927350364e-09</v>
       </c>
       <c r="D124" s="0">
-        <v>10743.186647949384</v>
+        <v>10284.373705800634</v>
       </c>
       <c r="E124" s="0">
-        <v>5.6440693806919969e-14</v>
+        <v>1.0629823927350364e-09</v>
       </c>
       <c r="F124" s="0"/>
     </row>
@@ -20499,13 +20499,13 @@
         <v>124</v>
       </c>
       <c r="C125" s="0">
-        <v>1.3421955684192085e-14</v>
+        <v>3.5924022132575777e-10</v>
       </c>
       <c r="D125" s="0">
-        <v>10690.248447885526</v>
+        <v>10252.304760199599</v>
       </c>
       <c r="E125" s="0">
-        <v>1.3421955684192085e-14</v>
+        <v>3.5924022132575777e-10</v>
       </c>
       <c r="F125" s="0"/>
     </row>
@@ -20517,13 +20517,13 @@
         <v>125</v>
       </c>
       <c r="C126" s="0">
-        <v>3.1124181387168634e-15</v>
+        <v>1.1912172287352676e-10</v>
       </c>
       <c r="D126" s="0">
-        <v>10637.977807131869</v>
+        <v>10234.6420540199</v>
       </c>
       <c r="E126" s="0">
-        <v>3.1124181387168634e-15</v>
+        <v>1.1912172287352676e-10</v>
       </c>
       <c r="F126" s="0"/>
     </row>
@@ -20535,13 +20535,13 @@
         <v>126</v>
       </c>
       <c r="C127" s="0">
-        <v>7.0378297226840151e-16</v>
+        <v>3.875646011735408e-11</v>
       </c>
       <c r="D127" s="0">
-        <v>10586.389344168485</v>
+        <v>10226.689008856214</v>
       </c>
       <c r="E127" s="0">
-        <v>7.0378297226840151e-16</v>
+        <v>3.875646011735408e-11</v>
       </c>
       <c r="F127" s="0"/>
     </row>
@@ -20553,13 +20553,13 @@
         <v>127</v>
       </c>
       <c r="C128" s="0">
-        <v>1.5518089515630778e-16</v>
+        <v>1.2372126925737762e-11</v>
       </c>
       <c r="D128" s="0">
-        <v>10535.497677475445</v>
+        <v>10223.262685605572</v>
       </c>
       <c r="E128" s="0">
-        <v>1.5518089515630778e-16</v>
+        <v>1.2372126925737762e-11</v>
       </c>
       <c r="F128" s="0"/>
     </row>
@@ -20571,13 +20571,13 @@
         <v>128</v>
       </c>
       <c r="C129" s="0">
-        <v>3.3365407299254555e-17</v>
+        <v>3.8751788998075539e-12</v>
       </c>
       <c r="D129" s="0">
-        <v>10485.317425532823</v>
+        <v>10221.077527163803</v>
       </c>
       <c r="E129" s="0">
-        <v>3.3365407299254555e-17</v>
+        <v>3.8751788998075539e-12</v>
       </c>
       <c r="F129" s="0"/>
     </row>
@@ -20589,13 +20589,13 @@
         <v>129</v>
       </c>
       <c r="C130" s="0">
-        <v>6.9954118610319157e-18</v>
+        <v>1.1909301033153628e-12</v>
       </c>
       <c r="D130" s="0">
-        <v>10435.858631669769</v>
+        <v>10218.342515493718</v>
       </c>
       <c r="E130" s="0">
-        <v>6.9954118610319157e-18</v>
+        <v>1.1909301033153628e-12</v>
       </c>
       <c r="F130" s="0"/>
     </row>
@@ -20607,13 +20607,13 @@
         <v>130</v>
       </c>
       <c r="C131" s="0">
-        <v>1.4301738326254902e-18</v>
+        <v>3.5911034478291475e-13</v>
       </c>
       <c r="D131" s="0">
-        <v>10387.10944881783</v>
+        <v>10212.863833842392</v>
       </c>
       <c r="E131" s="0">
-        <v>1.4301738326254902e-18</v>
+        <v>3.5911034478291475e-13</v>
       </c>
       <c r="F131" s="0"/>
     </row>
@@ -20625,13 +20625,13 @@
         <v>131</v>
       </c>
       <c r="C132" s="0">
-        <v>2.8511695654540002e-19</v>
+        <v>1.0624700219005648e-13</v>
       </c>
       <c r="D132" s="0">
-        <v>10339.036592512619</v>
+        <v>10202.863125562</v>
       </c>
       <c r="E132" s="0">
-        <v>2.8511695654540002e-19</v>
+        <v>1.0624700219005648e-13</v>
       </c>
       <c r="F132" s="0"/>
     </row>
@@ -20643,13 +20643,13 @@
         <v>132</v>
       </c>
       <c r="C133" s="0">
-        <v>5.5426307356968337e-20</v>
+        <v>3.0842713567129259e-14</v>
       </c>
       <c r="D133" s="0">
-        <v>10291.591512755171</v>
+        <v>10189.058914761908</v>
       </c>
       <c r="E133" s="0">
-        <v>5.5426307356968337e-20</v>
+        <v>3.0842713567129259e-14</v>
       </c>
       <c r="F133" s="0"/>
     </row>
@@ -20661,13 +20661,13 @@
         <v>133</v>
       </c>
       <c r="C134" s="0">
-        <v>1.0506728869140625e-20</v>
+        <v>8.7848753301219588e-15</v>
       </c>
       <c r="D134" s="0">
-        <v>10244.714796328035</v>
+        <v>10175.313135776163</v>
       </c>
       <c r="E134" s="0">
-        <v>1.0506728869140625e-20</v>
+        <v>8.7848753301219588e-15</v>
       </c>
       <c r="F134" s="0"/>
     </row>
@@ -20679,13 +20679,13 @@
         <v>134</v>
       </c>
       <c r="C135" s="0">
-        <v>1.9421277112654674e-21</v>
+        <v>2.4550805800262209e-15</v>
       </c>
       <c r="D135" s="0">
-        <v>10198.336958392563</v>
+        <v>10165.700105839353</v>
       </c>
       <c r="E135" s="0">
-        <v>1.9421277112654674e-21</v>
+        <v>2.4550805800262209e-15</v>
       </c>
       <c r="F135" s="0"/>
     </row>
@@ -20697,13 +20697,13 @@
         <v>135</v>
       </c>
       <c r="C136" s="0">
-        <v>3.5006341495976e-22</v>
+        <v>6.7319832352107235e-16</v>
       </c>
       <c r="D136" s="0">
-        <v>10152.379675222988</v>
+        <v>10162.11814031533</v>
       </c>
       <c r="E136" s="0">
-        <v>3.5006341495976e-22</v>
+        <v>6.7319832352107235e-16</v>
       </c>
       <c r="F136" s="0"/>
     </row>
@@ -20715,13 +20715,13 @@
         <v>136</v>
       </c>
       <c r="C137" s="0">
-        <v>6.1528219194193919e-23</v>
+        <v>1.8112042431964654e-16</v>
       </c>
       <c r="D137" s="0">
-        <v>10106.759284342141</v>
+        <v>10164.056620388001</v>
       </c>
       <c r="E137" s="0">
-        <v>6.1528219194193919e-23</v>
+        <v>1.8112042431964654e-16</v>
       </c>
       <c r="F137" s="0"/>
     </row>
@@ -20733,13 +20733,13 @@
         <v>137</v>
       </c>
       <c r="C138" s="0">
-        <v>1.0545341445013801e-23</v>
+        <v>4.7812224993939601e-17</v>
       </c>
       <c r="D138" s="0">
-        <v>10061.38937767461</v>
+        <v>10166.776524183846</v>
       </c>
       <c r="E138" s="0">
-        <v>1.0545341445013801e-23</v>
+        <v>4.7812224993939601e-17</v>
       </c>
       <c r="F138" s="0"/>
     </row>
@@ -20751,13 +20751,13 @@
         <v>138</v>
       </c>
       <c r="C139" s="0">
-        <v>1.7624046386634013e-24</v>
+        <v>1.2383904907126088e-17</v>
       </c>
       <c r="D139" s="0">
-        <v>10016.185705068547</v>
+        <v>10161.560080026857</v>
       </c>
       <c r="E139" s="0">
-        <v>1.7624046386634013e-24</v>
+        <v>1.2383904907126088e-17</v>
       </c>
       <c r="F139" s="0"/>
     </row>
@@ -20769,13 +20769,13 @@
         <v>139</v>
       </c>
       <c r="C140" s="0">
-        <v>2.8721643577591834e-25</v>
+        <v>3.1471930889906665e-18</v>
       </c>
       <c r="D140" s="0">
-        <v>9971.074742403036</v>
+        <v>10140.046501478977</v>
       </c>
       <c r="E140" s="0">
-        <v>2.8721643577591834e-25</v>
+        <v>3.1471930889906665e-18</v>
       </c>
       <c r="F140" s="0"/>
     </row>
@@ -20787,13 +20787,13 @@
         <v>140</v>
       </c>
       <c r="C141" s="0">
-        <v>4.5642731827608987e-26</v>
+        <v>7.8475898297606653e-19</v>
       </c>
       <c r="D141" s="0">
-        <v>9926.0047620490041</v>
+        <v>10102.241711840516</v>
       </c>
       <c r="E141" s="0">
-        <v>4.5642731827608987e-26</v>
+        <v>7.8475898297606653e-19</v>
       </c>
       <c r="F141" s="0"/>
     </row>

</xml_diff>